<commit_message>
Created testSortProductsInProductPage test case
</commit_message>
<xml_diff>
--- a/src/test/resources/nopCommerce_FrontEnd_TestCases.xlsx
+++ b/src/test/resources/nopCommerce_FrontEnd_TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharmin Zaman\IdeaProjects\nopCommerce\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehna\nopCommerce\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB2656D-B895-4FA9-96D7-AA63753FB65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED053F0B-F6F1-44B0-8365-992CEF7447E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{5BE317AF-6064-4EB0-BD7F-9D2C2ECF4852}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="10140" activeTab="3" xr2:uid="{5BE317AF-6064-4EB0-BD7F-9D2C2ECF4852}"/>
   </bookViews>
   <sheets>
     <sheet name="Sharmin" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="101">
   <si>
     <t>Test Case</t>
   </si>
@@ -350,6 +350,39 @@
   </si>
   <si>
     <t>Test: Add to wishlist</t>
+  </si>
+  <si>
+    <t>Sort shoe prices from low to high</t>
+  </si>
+  <si>
+    <t>Hover over apparel menu option</t>
+  </si>
+  <si>
+    <t>Click on shoes option link</t>
+  </si>
+  <si>
+    <t>Click on sort by dropdown</t>
+  </si>
+  <si>
+    <t>Click on prices low to high option</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Land on frontend homepage</t>
+  </si>
+  <si>
+    <t>Apparel subcategory options appear</t>
+  </si>
+  <si>
+    <t>Land on shoes product page</t>
+  </si>
+  <si>
+    <t>Sort by options appear</t>
+  </si>
+  <si>
+    <t>Products are sorted by low to high prices</t>
   </si>
 </sst>
 </file>
@@ -519,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -579,6 +612,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -898,7 +936,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -944,7 +982,7 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="30" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1617,9 +1655,10 @@
   <hyperlinks>
     <hyperlink ref="D13" r:id="rId1" xr:uid="{92E303BA-BCFD-48EF-8525-D40B11FD7176}"/>
     <hyperlink ref="D21" r:id="rId2" display="zamansharmin000@gmail.com" xr:uid="{DB3C4841-5E61-4484-A613-DBF4C08C117C}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{CFEF3CA7-E2EC-4D70-AD5D-A331AE49AE5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1716,20 +1755,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7359425C-0B41-4C71-89B4-A9A79147A9A2}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1752,7 +1793,83 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A2:A6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4AB0E2C5-6792-4BE8-811D-A53D5205946A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1847,7 +1964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A569904C-E53A-44CB-AA02-0DBE012274D9}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>

</xml_diff>